<commit_message>
add a comment about php version
</commit_message>
<xml_diff>
--- a/tests/data/basic.xlsx
+++ b/tests/data/basic.xlsx
@@ -43,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -64,6 +65,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,12 +110,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -249,13 +255,13 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>